<commit_message>
Better handling of decimals
</commit_message>
<xml_diff>
--- a/test_data/format.xlsx
+++ b/test_data/format.xlsx
@@ -32,8 +32,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.00E+00"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -100,9 +102,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -122,10 +136,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -152,9 +166,16 @@
       <c r="E1" s="0" t="n">
         <v>0.000130316679844963</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="n">
+        <v>2.66666156237642</v>
+      </c>
+      <c r="G1" s="2" t="n">
+        <v>2.66666156237642</v>
+      </c>
+      <c r="H1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="I1" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Function to reproduce excel digits (will be discarded)
</commit_message>
<xml_diff>
--- a/test_data/format.xlsx
+++ b/test_data/format.xlsx
@@ -136,17 +136,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.84"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.59"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -164,7 +166,7 @@
         <v>60</v>
       </c>
       <c r="E1" s="0" t="n">
-        <v>0.000130316679844963</v>
+        <v>0.0148290494731055</v>
       </c>
       <c r="F1" s="1" t="n">
         <v>2.66666156237642</v>
@@ -172,10 +174,18 @@
       <c r="G1" s="2" t="n">
         <v>2.66666156237642</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="0" t="n">
+        <v>-0.00360507125957782</v>
+      </c>
+      <c r="I1" s="3" t="n">
+        <v>0.000338847568184501</v>
+      </c>
+      <c r="J1" s="0" t="n">
+        <v>-0.0867370786746085</v>
+      </c>
+      <c r="K1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Add no-format options - extend README
</commit_message>
<xml_diff>
--- a/test_data/format.xlsx
+++ b/test_data/format.xlsx
@@ -32,10 +32,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
+    <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="169" formatCode="0.00%"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -102,7 +105,11 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -117,6 +124,18 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -136,10 +155,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -155,7 +174,7 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="n">
+      <c r="B1" s="1" t="n">
         <v>2.66666156237642</v>
       </c>
       <c r="C1" s="0" t="n">
@@ -168,22 +187,31 @@
       <c r="E1" s="0" t="n">
         <v>0.0148290494731055</v>
       </c>
-      <c r="F1" s="1" t="n">
+      <c r="F1" s="2" t="n">
         <v>2.66666156237642</v>
       </c>
-      <c r="G1" s="2" t="n">
-        <v>2.66666156237642</v>
+      <c r="G1" s="3" t="n">
+        <v>200.666661562376</v>
       </c>
       <c r="H1" s="0" t="n">
         <v>-0.00360507125957782</v>
       </c>
-      <c r="I1" s="3" t="n">
+      <c r="I1" s="4" t="n">
         <v>0.000338847568184501</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>-0.0867370786746085</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="5" t="n">
+        <v>43911</v>
+      </c>
+      <c r="L1" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="M1" s="7" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="N1" s="0" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>